<commit_message>
Done with Task 3
</commit_message>
<xml_diff>
--- a/Charts and Data for Lab 3.xlsx
+++ b/Charts and Data for Lab 3.xlsx
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,6 +1570,10 @@
       <c r="B4">
         <f>(1951.68+1953.69+1949.28+1931.42)/4</f>
         <v>1946.5174999999999</v>
+      </c>
+      <c r="C4">
+        <f>(1967.31+1979.68+1966.46+1981.93)/4</f>
+        <v>1973.845</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>